<commit_message>
adding updated files on 15 march 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishal\git\dataDrivenSeleniumRepo\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD5835-3CD8-4EF9-A5BC-42BA50080C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D25F23F-FCD0-4719-AD1F-35055C7F6318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>postcode</t>
   </si>
@@ -34,9 +35,6 @@
     <t>firstname</t>
   </si>
   <si>
-    <t>lastanme</t>
-  </si>
-  <si>
     <t>Arora</t>
   </si>
   <si>
@@ -56,6 +54,48 @@
   </si>
   <si>
     <t>Rupee</t>
+  </si>
+  <si>
+    <t>Vishal</t>
+  </si>
+  <si>
+    <t>Soniya</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Sehgal</t>
+  </si>
+  <si>
+    <t>Raman Arora</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>lastname</t>
   </si>
 </sst>
 </file>
@@ -372,8 +412,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45106967-17DD-44FC-A096-77682160923D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>35435</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>35435</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>35435</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>35435</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7B92CA-BCDE-45A3-84BE-0D02961B8B54}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -381,66 +574,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>35435</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7B92CA-BCDE-45A3-84BE-0D02961B8B54}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>